<commit_message>
adjusting roles so the workflow runs without issues
</commit_message>
<xml_diff>
--- a/nes-lter-attune-transect-info.xlsx
+++ b/nes-lter-attune-transect-info.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20383"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfutrelle\Documents\GitHub\nes-lter-attune-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B15586-F1B0-4F63-8721-66262B20539A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22788" windowHeight="8592" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22788" windowHeight="8592" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="5" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="93">
   <si>
     <t>keyword</t>
   </si>
@@ -302,12 +303,15 @@
   </si>
   <si>
     <t>jfutrelle@whoi.edu</t>
+  </si>
+  <si>
+    <t>PI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -620,19 +624,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="7" width="27.21875" style="1" customWidth="1"/>
+    <col min="1" max="7" width="27.20703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -655,7 +659,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -666,7 +670,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -686,7 +690,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -706,7 +710,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -726,7 +730,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>71</v>
       </c>
@@ -746,7 +750,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>72</v>
       </c>
@@ -766,7 +770,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -786,7 +790,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -806,7 +810,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>75</v>
       </c>
@@ -830,19 +834,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -874,7 +878,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -894,7 +898,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="H2" t="s">
         <v>17</v>
@@ -906,7 +910,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -932,7 +936,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -961,7 +965,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -987,7 +991,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1010,7 +1014,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1033,7 +1037,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>89</v>
       </c>
@@ -1045,6 +1049,9 @@
       </c>
       <c r="E8" t="s">
         <v>91</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
       </c>
       <c r="H8" t="s">
         <v>17</v>
@@ -1062,19 +1069,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.89453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1082,7 +1089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1090,7 +1097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1098,7 +1105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1106,7 +1113,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1114,7 +1121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1122,7 +1129,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1130,7 +1137,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1138,7 +1145,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1146,7 +1153,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -1154,7 +1161,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -1162,7 +1169,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -1170,7 +1177,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>58</v>
       </c>

</xml_diff>